<commit_message>
Working on a control to hold graphics drawing with auto scrolling
</commit_message>
<xml_diff>
--- a/MazeBuilder/Analysis.xlsx
+++ b/MazeBuilder/Analysis.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="21075" windowHeight="8250"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="21075" windowHeight="8250" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,8 +13,9 @@
   </sheets>
   <definedNames>
     <definedName name="GenerationTimes" localSheetId="0">Sheet1!$A$1:$B$100</definedName>
+    <definedName name="GenerationTimes" localSheetId="1">Sheet2!$A$1:$B$100</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -28,12 +29,28 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="2" name="GenerationTimes1" type="6" refreshedVersion="4" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\ws\MilesAndJon\MazeBuilder\MazeBuilder\GenerationTimes.txt" tab="0" space="1" comma="1" consecutive="1">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Total</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,17 +87,34 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -89,6 +123,7 @@
           </c:marker>
           <c:trendline>
             <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout/>
@@ -299,34 +334,51 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="50319360"/>
-        <c:axId val="50320896"/>
+        <c:smooth val="0"/>
+        <c:axId val="187888128"/>
+        <c:axId val="161944064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="50319360"/>
+        <c:axId val="187888128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50320896"/>
+        <c:crossAx val="161944064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50320896"/>
+        <c:axId val="161944064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50319360"/>
+        <c:crossAx val="187888128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -334,8 +386,426 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$1:$B$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>1.2999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.1000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.4000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.8000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.11899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.14199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.109</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.14199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.191</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.20300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.23799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.249</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.29799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.34200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.30099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.40300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.39300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.442</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.51800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.46100000000000002</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.497</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.58799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.52300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.65800000000000003</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.61799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.68600000000000005</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.58499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.72899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.77600000000000002</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.67400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.78200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.73199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.82199999999999995</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.83299999999999996</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.91400000000000003</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.84899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.96399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.90100000000000002</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.95499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.0309999999999999</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.93200000000000005</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.1100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.97799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.081</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.0649999999999999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.1719999999999999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.01</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.17</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.179</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.194</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.216</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.2549999999999999</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.3029999999999999</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.254</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.3819999999999999</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.252</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.4330000000000001</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.3839999999999999</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.367</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.4890000000000001</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.399</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.488</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.5249999999999999</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.4430000000000001</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.68</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.4670000000000001</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.6559999999999999</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1.653</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1.5940000000000001</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1.675</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1.8149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1.7250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1.698</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1.929</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1.804</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1.8149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1.77</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1.8520000000000001</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1.9059999999999999</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1.9059999999999999</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1.946</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2.0539999999999998</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1.9390000000000001</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2.149</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1.9970000000000001</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2.11</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2.1059999999999999</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2.0830000000000002</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2.125</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2.1070000000000002</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2.3330000000000002</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2.0310000000000001</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2.2759999999999998</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2.323</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2.1549999999999998</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2.3570000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="43469824"/>
+        <c:axId val="56214080"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="43469824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="56214080"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="56214080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="43469824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -380,8 +850,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GenerationTimes" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GenerationTimes" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -459,6 +968,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -493,6 +1003,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -668,20 +1179,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>10000</v>
       </c>
@@ -689,7 +1200,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20000</v>
       </c>
@@ -697,7 +1208,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>30000</v>
       </c>
@@ -705,7 +1216,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>40000</v>
       </c>
@@ -713,7 +1224,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>50000</v>
       </c>
@@ -721,7 +1232,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>60000</v>
       </c>
@@ -729,7 +1240,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>70000</v>
       </c>
@@ -737,7 +1248,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>80000</v>
       </c>
@@ -745,7 +1256,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>90000</v>
       </c>
@@ -753,7 +1264,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>100000</v>
       </c>
@@ -761,7 +1272,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>110000</v>
       </c>
@@ -769,7 +1280,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>120000</v>
       </c>
@@ -777,7 +1288,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>130000</v>
       </c>
@@ -785,7 +1296,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>140000</v>
       </c>
@@ -793,7 +1304,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>150000</v>
       </c>
@@ -801,7 +1312,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>160000</v>
       </c>
@@ -809,7 +1320,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>170000</v>
       </c>
@@ -817,7 +1328,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>180000</v>
       </c>
@@ -825,7 +1336,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>190000</v>
       </c>
@@ -833,7 +1344,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>200000</v>
       </c>
@@ -841,7 +1352,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>210000</v>
       </c>
@@ -849,7 +1360,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>220000</v>
       </c>
@@ -857,7 +1368,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>230000</v>
       </c>
@@ -865,7 +1376,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>240000</v>
       </c>
@@ -873,7 +1384,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>250000</v>
       </c>
@@ -881,7 +1392,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>260000</v>
       </c>
@@ -889,7 +1400,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>270000</v>
       </c>
@@ -897,7 +1408,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>280000</v>
       </c>
@@ -905,7 +1416,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>290000</v>
       </c>
@@ -913,7 +1424,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>300000</v>
       </c>
@@ -921,7 +1432,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>310000</v>
       </c>
@@ -929,7 +1440,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>320000</v>
       </c>
@@ -937,7 +1448,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>330000</v>
       </c>
@@ -945,7 +1456,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>340000</v>
       </c>
@@ -953,7 +1464,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>350000</v>
       </c>
@@ -961,7 +1472,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>360000</v>
       </c>
@@ -969,7 +1480,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>370000</v>
       </c>
@@ -977,7 +1488,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>380000</v>
       </c>
@@ -985,7 +1496,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>390000</v>
       </c>
@@ -993,7 +1504,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>400000</v>
       </c>
@@ -1001,7 +1512,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>410000</v>
       </c>
@@ -1009,7 +1520,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>420000</v>
       </c>
@@ -1017,7 +1528,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>430000</v>
       </c>
@@ -1025,7 +1536,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>440000</v>
       </c>
@@ -1033,7 +1544,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>450000</v>
       </c>
@@ -1041,7 +1552,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>460000</v>
       </c>
@@ -1049,7 +1560,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>470000</v>
       </c>
@@ -1057,7 +1568,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>480000</v>
       </c>
@@ -1065,7 +1576,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>490000</v>
       </c>
@@ -1073,7 +1584,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>500000</v>
       </c>
@@ -1081,7 +1592,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>510000</v>
       </c>
@@ -1089,7 +1600,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>520000</v>
       </c>
@@ -1097,7 +1608,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>530000</v>
       </c>
@@ -1105,7 +1616,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>540000</v>
       </c>
@@ -1113,7 +1624,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>550000</v>
       </c>
@@ -1121,7 +1632,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>560000</v>
       </c>
@@ -1129,7 +1640,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>570000</v>
       </c>
@@ -1137,7 +1648,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>580000</v>
       </c>
@@ -1145,7 +1656,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>590000</v>
       </c>
@@ -1153,7 +1664,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>600000</v>
       </c>
@@ -1161,7 +1672,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>610000</v>
       </c>
@@ -1169,7 +1680,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>620000</v>
       </c>
@@ -1177,7 +1688,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>630000</v>
       </c>
@@ -1185,7 +1696,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>640000</v>
       </c>
@@ -1193,7 +1704,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>650000</v>
       </c>
@@ -1201,7 +1712,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>660000</v>
       </c>
@@ -1209,7 +1720,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>670000</v>
       </c>
@@ -1217,7 +1728,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>680000</v>
       </c>
@@ -1225,7 +1736,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>690000</v>
       </c>
@@ -1233,7 +1744,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>700000</v>
       </c>
@@ -1241,7 +1752,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>710000</v>
       </c>
@@ -1249,7 +1760,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>720000</v>
       </c>
@@ -1257,7 +1768,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>730000</v>
       </c>
@@ -1265,7 +1776,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>740000</v>
       </c>
@@ -1273,7 +1784,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>750000</v>
       </c>
@@ -1281,7 +1792,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>760000</v>
       </c>
@@ -1289,7 +1800,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>770000</v>
       </c>
@@ -1297,7 +1808,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>780000</v>
       </c>
@@ -1305,7 +1816,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>790000</v>
       </c>
@@ -1313,7 +1824,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>800000</v>
       </c>
@@ -1321,7 +1832,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>810000</v>
       </c>
@@ -1329,7 +1840,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>820000</v>
       </c>
@@ -1337,7 +1848,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>830000</v>
       </c>
@@ -1345,7 +1856,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>840000</v>
       </c>
@@ -1353,7 +1864,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>850000</v>
       </c>
@@ -1361,7 +1872,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>860000</v>
       </c>
@@ -1369,7 +1880,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>870000</v>
       </c>
@@ -1377,7 +1888,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>880000</v>
       </c>
@@ -1385,7 +1896,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>890000</v>
       </c>
@@ -1393,7 +1904,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>900000</v>
       </c>
@@ -1401,7 +1912,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>910000</v>
       </c>
@@ -1409,7 +1920,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>920000</v>
       </c>
@@ -1417,7 +1928,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>930000</v>
       </c>
@@ -1425,7 +1936,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>940000</v>
       </c>
@@ -1433,7 +1944,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>950000</v>
       </c>
@@ -1441,7 +1952,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>960000</v>
       </c>
@@ -1449,7 +1960,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>970000</v>
       </c>
@@ -1457,7 +1968,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>980000</v>
       </c>
@@ -1465,7 +1976,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>990000</v>
       </c>
@@ -1473,7 +1984,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>1000000</v>
       </c>
@@ -1488,24 +1999,841 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>10000</v>
+      </c>
+      <c r="B1">
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>20000</v>
+      </c>
+      <c r="B2">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>30000</v>
+      </c>
+      <c r="B3">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>40000</v>
+      </c>
+      <c r="B4">
+        <v>4.1000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>50000</v>
+      </c>
+      <c r="B5">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>60000</v>
+      </c>
+      <c r="B6">
+        <v>5.8000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>70000</v>
+      </c>
+      <c r="B7">
+        <v>0.11899999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>80000</v>
+      </c>
+      <c r="B8">
+        <v>0.14199999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>90000</v>
+      </c>
+      <c r="B9">
+        <v>0.109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>100000</v>
+      </c>
+      <c r="B10">
+        <v>0.14199999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>110000</v>
+      </c>
+      <c r="B11">
+        <v>0.191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>120000</v>
+      </c>
+      <c r="B12">
+        <v>0.20300000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>130000</v>
+      </c>
+      <c r="B13">
+        <v>0.23799999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>140000</v>
+      </c>
+      <c r="B14">
+        <v>0.249</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>150000</v>
+      </c>
+      <c r="B15">
+        <v>0.29799999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>160000</v>
+      </c>
+      <c r="B16">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>170000</v>
+      </c>
+      <c r="B17">
+        <v>0.34200000000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>180000</v>
+      </c>
+      <c r="B18">
+        <v>0.30099999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>190000</v>
+      </c>
+      <c r="B19">
+        <v>0.40300000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>200000</v>
+      </c>
+      <c r="B20">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>210000</v>
+      </c>
+      <c r="B21">
+        <v>0.39300000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>220000</v>
+      </c>
+      <c r="B22">
+        <v>0.442</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>230000</v>
+      </c>
+      <c r="B23">
+        <v>0.51800000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>240000</v>
+      </c>
+      <c r="B24">
+        <v>0.46100000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>250000</v>
+      </c>
+      <c r="B25">
+        <v>0.497</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>260000</v>
+      </c>
+      <c r="B26">
+        <v>0.58799999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>270000</v>
+      </c>
+      <c r="B27">
+        <v>0.52300000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>280000</v>
+      </c>
+      <c r="B28">
+        <v>0.65800000000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>290000</v>
+      </c>
+      <c r="B29">
+        <v>0.61799999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>300000</v>
+      </c>
+      <c r="B30">
+        <v>0.68600000000000005</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>310000</v>
+      </c>
+      <c r="B31">
+        <v>0.58499999999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>320000</v>
+      </c>
+      <c r="B32">
+        <v>0.72899999999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>330000</v>
+      </c>
+      <c r="B33">
+        <v>0.77600000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>340000</v>
+      </c>
+      <c r="B34">
+        <v>0.67400000000000004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>350000</v>
+      </c>
+      <c r="B35">
+        <v>0.78200000000000003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>360000</v>
+      </c>
+      <c r="B36">
+        <v>0.73199999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>370000</v>
+      </c>
+      <c r="B37">
+        <v>0.82199999999999995</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>380000</v>
+      </c>
+      <c r="B38">
+        <v>0.83299999999999996</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>390000</v>
+      </c>
+      <c r="B39">
+        <v>0.91400000000000003</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>400000</v>
+      </c>
+      <c r="B40">
+        <v>0.84899999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>410000</v>
+      </c>
+      <c r="B41">
+        <v>0.96399999999999997</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>420000</v>
+      </c>
+      <c r="B42">
+        <v>0.90100000000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>430000</v>
+      </c>
+      <c r="B43">
+        <v>0.95499999999999996</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>440000</v>
+      </c>
+      <c r="B44">
+        <v>1.0309999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>450000</v>
+      </c>
+      <c r="B45">
+        <v>0.93200000000000005</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>460000</v>
+      </c>
+      <c r="B46">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>470000</v>
+      </c>
+      <c r="B47">
+        <v>0.97799999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>480000</v>
+      </c>
+      <c r="B48">
+        <v>1.081</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>490000</v>
+      </c>
+      <c r="B49">
+        <v>1.0649999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>500000</v>
+      </c>
+      <c r="B50">
+        <v>1.1719999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>510000</v>
+      </c>
+      <c r="B51">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>520000</v>
+      </c>
+      <c r="B52">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>530000</v>
+      </c>
+      <c r="B53">
+        <v>1.179</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>540000</v>
+      </c>
+      <c r="B54">
+        <v>1.194</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>550000</v>
+      </c>
+      <c r="B55">
+        <v>1.216</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>560000</v>
+      </c>
+      <c r="B56">
+        <v>1.2549999999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>570000</v>
+      </c>
+      <c r="B57">
+        <v>1.3029999999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>580000</v>
+      </c>
+      <c r="B58">
+        <v>1.254</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>590000</v>
+      </c>
+      <c r="B59">
+        <v>1.3819999999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>600000</v>
+      </c>
+      <c r="B60">
+        <v>1.252</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>610000</v>
+      </c>
+      <c r="B61">
+        <v>1.4330000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>620000</v>
+      </c>
+      <c r="B62">
+        <v>1.3839999999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>630000</v>
+      </c>
+      <c r="B63">
+        <v>1.367</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>640000</v>
+      </c>
+      <c r="B64">
+        <v>1.4890000000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>650000</v>
+      </c>
+      <c r="B65">
+        <v>1.399</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>660000</v>
+      </c>
+      <c r="B66">
+        <v>1.488</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>670000</v>
+      </c>
+      <c r="B67">
+        <v>1.5249999999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>680000</v>
+      </c>
+      <c r="B68">
+        <v>1.4430000000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>690000</v>
+      </c>
+      <c r="B69">
+        <v>1.68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>700000</v>
+      </c>
+      <c r="B70">
+        <v>1.4670000000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>710000</v>
+      </c>
+      <c r="B71">
+        <v>1.6559999999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>720000</v>
+      </c>
+      <c r="B72">
+        <v>1.653</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>730000</v>
+      </c>
+      <c r="B73">
+        <v>1.5940000000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>740000</v>
+      </c>
+      <c r="B74">
+        <v>1.675</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>750000</v>
+      </c>
+      <c r="B75">
+        <v>1.8149999999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>760000</v>
+      </c>
+      <c r="B76">
+        <v>1.7250000000000001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>770000</v>
+      </c>
+      <c r="B77">
+        <v>1.698</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>780000</v>
+      </c>
+      <c r="B78">
+        <v>1.929</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>790000</v>
+      </c>
+      <c r="B79">
+        <v>1.804</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>800000</v>
+      </c>
+      <c r="B80">
+        <v>1.8149999999999999</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>810000</v>
+      </c>
+      <c r="B81">
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>820000</v>
+      </c>
+      <c r="B82">
+        <v>1.8520000000000001</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>830000</v>
+      </c>
+      <c r="B83">
+        <v>1.9059999999999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>840000</v>
+      </c>
+      <c r="B84">
+        <v>1.9059999999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>850000</v>
+      </c>
+      <c r="B85">
+        <v>1.946</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>860000</v>
+      </c>
+      <c r="B86">
+        <v>2.0539999999999998</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>870000</v>
+      </c>
+      <c r="B87">
+        <v>1.9390000000000001</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>880000</v>
+      </c>
+      <c r="B88">
+        <v>2.149</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>890000</v>
+      </c>
+      <c r="B89">
+        <v>1.9970000000000001</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>900000</v>
+      </c>
+      <c r="B90">
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>910000</v>
+      </c>
+      <c r="B91">
+        <v>2.1059999999999999</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>920000</v>
+      </c>
+      <c r="B92">
+        <v>2.0830000000000002</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>930000</v>
+      </c>
+      <c r="B93">
+        <v>2.125</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>940000</v>
+      </c>
+      <c r="B94">
+        <v>2.1070000000000002</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>950000</v>
+      </c>
+      <c r="B95">
+        <v>2.3330000000000002</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>960000</v>
+      </c>
+      <c r="B96">
+        <v>2.0310000000000001</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>970000</v>
+      </c>
+      <c r="B97">
+        <v>2.2759999999999998</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>980000</v>
+      </c>
+      <c r="B98">
+        <v>2.323</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>990000</v>
+      </c>
+      <c r="B99">
+        <v>2.1549999999999998</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>1000000</v>
+      </c>
+      <c r="B100">
+        <v>2.3570000000000002</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>0</v>
+      </c>
+      <c r="B101">
+        <f>SUM(B1:B100)</f>
+        <v>112.67099999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>